<commit_message>
Urendeclaratie toegeveogd + Systeemtestplan
</commit_message>
<xml_diff>
--- a/Urendeclaratie.xlsx
+++ b/Urendeclaratie.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>TAKEN</t>
   </si>
@@ -117,7 +117,7 @@
     <t>presentatie</t>
   </si>
   <si>
-    <t>tesplan 1:00:00</t>
+    <t>Systeem testplan</t>
   </si>
 </sst>
 </file>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -274,6 +274,8 @@
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -546,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,13 +558,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" style="1" customWidth="1"/>
     <col min="2" max="9" width="18.28515625" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -668,7 +670,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="7">
-        <v>4.1666666666666664E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7">
@@ -721,7 +723,9 @@
       <c r="B7" s="7">
         <v>0</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7">
+        <v>1.7361111111111112E-2</v>
+      </c>
       <c r="D7" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -748,7 +752,9 @@
       <c r="B8" s="7">
         <v>0</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D8" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -775,19 +781,19 @@
         <v>4.75</v>
       </c>
       <c r="C9" s="13">
-        <f t="shared" ref="C9:I9" si="0">SUM(C3:C8)*24</f>
-        <v>7.3333333333333321</v>
+        <f t="shared" ref="C9" si="0">SUM(C3:C8)*24</f>
+        <v>7.0833333333333321</v>
       </c>
       <c r="D9" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D9:I9" si="1">SUM(D3:D8)*24</f>
         <v>6.9999999999999991</v>
       </c>
       <c r="E9" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.9999999999999991</v>
       </c>
       <c r="F9" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.1666666666666661</v>
       </c>
       <c r="G9" s="13">
@@ -795,11 +801,11 @@
         <v>6.1666666666666661</v>
       </c>
       <c r="H9" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
       <c r="I9" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
@@ -892,6 +898,9 @@
       <c r="B14" s="9">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="C14" s="15">
+        <v>0</v>
+      </c>
       <c r="D14" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -910,6 +919,9 @@
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
+      <c r="C15" s="12">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E15" s="12">
         <v>0</v>
       </c>
@@ -929,19 +941,19 @@
         <v>6.5</v>
       </c>
       <c r="C16" s="13">
-        <f t="shared" ref="C16:I16" si="1">SUM(C10:C15)*24</f>
-        <v>5.9999999999999991</v>
+        <f t="shared" ref="C16" si="2">SUM(C10:C15)*24</f>
+        <v>6.1666666666666661</v>
       </c>
       <c r="D16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D16:I16" si="3">SUM(D10:D15)*24</f>
         <v>5.833333333333333</v>
       </c>
       <c r="E16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.9999999999999991</v>
       </c>
       <c r="F16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G16" s="13">
@@ -949,11 +961,11 @@
         <v>7.5</v>
       </c>
       <c r="H16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.833333333333334</v>
       </c>
     </row>
@@ -975,7 +987,9 @@
         <v>8</v>
       </c>
       <c r="B18" s="9"/>
-      <c r="C18" s="7"/>
+      <c r="C18" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D18" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -992,7 +1006,9 @@
         <v>9</v>
       </c>
       <c r="B19" s="9"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D19" s="7">
         <v>0.16666666666666666</v>
       </c>
@@ -1005,9 +1021,13 @@
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="B20" s="9"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D20" s="12"/>
       <c r="E20" s="7">
         <v>0</v>
@@ -1022,6 +1042,9 @@
         <v>28</v>
       </c>
       <c r="B21" s="9"/>
+      <c r="C21" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D21" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1038,6 +1061,9 @@
         <v>18</v>
       </c>
       <c r="B22" s="9"/>
+      <c r="C22" s="12">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="E22" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1055,19 +1081,19 @@
         <v>0</v>
       </c>
       <c r="C23" s="13">
-        <f t="shared" ref="C23" si="2">SUM(C17:C22)*24</f>
-        <v>0</v>
+        <f t="shared" ref="C23" si="4">SUM(C17:C22)*24</f>
+        <v>5.833333333333333</v>
       </c>
       <c r="D23" s="13">
-        <f t="shared" ref="D23" si="3">SUM(D17:D22)*24</f>
+        <f t="shared" ref="D23" si="5">SUM(D17:D22)*24</f>
         <v>5.9999999999999991</v>
       </c>
       <c r="E23" s="13">
-        <f t="shared" ref="E23" si="4">SUM(E17:E22)*24</f>
+        <f t="shared" ref="E23" si="6">SUM(E17:E22)*24</f>
         <v>5.9999999999999991</v>
       </c>
       <c r="F23" s="13">
-        <f t="shared" ref="F23" si="5">SUM(F17:F22)*24</f>
+        <f t="shared" ref="F23" si="7">SUM(F17:F22)*24</f>
         <v>0</v>
       </c>
       <c r="G23" s="13">
@@ -1075,11 +1101,11 @@
         <v>5.9999999999999991</v>
       </c>
       <c r="H23" s="13">
-        <f t="shared" ref="H23" si="6">SUM(H17:H22)*24</f>
+        <f t="shared" ref="H23" si="8">SUM(H17:H22)*24</f>
         <v>0</v>
       </c>
       <c r="I23" s="13">
-        <f t="shared" ref="I23" si="7">SUM(I17:I22)*24</f>
+        <f t="shared" ref="I23" si="9">SUM(I17:I22)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1101,7 +1127,9 @@
         <v>8</v>
       </c>
       <c r="B25" s="9"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D25" s="7"/>
       <c r="E25" s="12">
         <v>4.1666666666666664E-2</v>
@@ -1116,7 +1144,9 @@
         <v>9</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7">
         <v>0</v>
@@ -1131,7 +1161,9 @@
         <v>17</v>
       </c>
       <c r="B27" s="9"/>
-      <c r="C27" s="7"/>
+      <c r="C27" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12">
         <v>8.3333333333333329E-2</v>
@@ -1146,6 +1178,9 @@
         <v>29</v>
       </c>
       <c r="B28" s="9"/>
+      <c r="C28" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12">
         <v>0</v>
@@ -1160,6 +1195,9 @@
         <v>30</v>
       </c>
       <c r="B29" s="9"/>
+      <c r="C29" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E29" s="12">
         <v>0</v>
       </c>
@@ -1177,19 +1215,19 @@
         <v>0</v>
       </c>
       <c r="C30" s="13">
-        <f t="shared" ref="C30" si="8">SUM(C24:C29)*24</f>
-        <v>0</v>
+        <f t="shared" ref="C30" si="10">SUM(C24:C29)*24</f>
+        <v>2.5</v>
       </c>
       <c r="D30" s="13">
-        <f t="shared" ref="D30" si="9">SUM(D24:D29)*24</f>
+        <f t="shared" ref="D30" si="11">SUM(D24:D29)*24</f>
         <v>0</v>
       </c>
       <c r="E30" s="13">
-        <f t="shared" ref="E30" si="10">SUM(E24:E29)*24</f>
+        <f t="shared" ref="E30" si="12">SUM(E24:E29)*24</f>
         <v>3</v>
       </c>
       <c r="F30" s="13">
-        <f t="shared" ref="F30" si="11">SUM(F24:F29)*24</f>
+        <f t="shared" ref="F30" si="13">SUM(F24:F29)*24</f>
         <v>0</v>
       </c>
       <c r="G30" s="13">
@@ -1197,11 +1235,11 @@
         <v>3.5</v>
       </c>
       <c r="H30" s="13">
-        <f t="shared" ref="H30" si="12">SUM(H24:H29)*24</f>
+        <f t="shared" ref="H30" si="14">SUM(H24:H29)*24</f>
         <v>0</v>
       </c>
       <c r="I30" s="13">
-        <f t="shared" ref="I30" si="13">SUM(I24:I29)*24</f>
+        <f t="shared" ref="I30" si="15">SUM(I24:I29)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1223,7 +1261,9 @@
         <v>8</v>
       </c>
       <c r="B32" s="9"/>
-      <c r="C32" s="7"/>
+      <c r="C32" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D32" s="7"/>
       <c r="E32" s="12">
         <v>4.1666666666666664E-2</v>
@@ -1238,7 +1278,9 @@
         <v>9</v>
       </c>
       <c r="B33" s="9"/>
-      <c r="C33" s="7"/>
+      <c r="C33" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D33" s="7"/>
       <c r="E33" s="12">
         <v>0.16666666666666666</v>
@@ -1253,7 +1295,9 @@
         <v>17</v>
       </c>
       <c r="B34" s="9"/>
-      <c r="C34" s="7"/>
+      <c r="C34" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D34" s="12"/>
       <c r="E34" s="7">
         <v>0</v>
@@ -1268,6 +1312,9 @@
         <v>29</v>
       </c>
       <c r="B35" s="9"/>
+      <c r="C35" s="12">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12">
         <v>6.25E-2</v>
@@ -1282,6 +1329,9 @@
         <v>30</v>
       </c>
       <c r="B36" s="9"/>
+      <c r="C36" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E36" s="12">
         <v>0</v>
       </c>
@@ -1299,19 +1349,19 @@
         <v>0</v>
       </c>
       <c r="C37" s="13">
-        <f t="shared" ref="C37" si="14">SUM(C31:C36)*24</f>
-        <v>0</v>
+        <f t="shared" ref="C37" si="16">SUM(C31:C36)*24</f>
+        <v>7.1666666666666661</v>
       </c>
       <c r="D37" s="13">
-        <f t="shared" ref="D37" si="15">SUM(D31:D36)*24</f>
+        <f t="shared" ref="D37" si="17">SUM(D31:D36)*24</f>
         <v>0</v>
       </c>
       <c r="E37" s="13">
-        <f t="shared" ref="E37" si="16">SUM(E31:E36)*24</f>
+        <f t="shared" ref="E37" si="18">SUM(E31:E36)*24</f>
         <v>6.5</v>
       </c>
       <c r="F37" s="13">
-        <f t="shared" ref="F37" si="17">SUM(F31:F36)*24</f>
+        <f t="shared" ref="F37" si="19">SUM(F31:F36)*24</f>
         <v>0</v>
       </c>
       <c r="G37" s="13">
@@ -1319,11 +1369,11 @@
         <v>5.9999999999999991</v>
       </c>
       <c r="H37" s="13">
-        <f t="shared" ref="H37" si="18">SUM(H31:H36)*24</f>
+        <f t="shared" ref="H37" si="20">SUM(H31:H36)*24</f>
         <v>0</v>
       </c>
       <c r="I37" s="13">
-        <f t="shared" ref="I37" si="19">SUM(I31:I36)*24</f>
+        <f t="shared" ref="I37" si="21">SUM(I31:I36)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1345,7 +1395,9 @@
         <v>8</v>
       </c>
       <c r="B39" s="9"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D39" s="7"/>
       <c r="E39" s="12">
         <v>4.1666666666666664E-2</v>
@@ -1360,7 +1412,9 @@
         <v>9</v>
       </c>
       <c r="B40" s="9"/>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D40" s="7"/>
       <c r="E40" s="12">
         <v>0.16666666666666666</v>
@@ -1375,7 +1429,9 @@
         <v>17</v>
       </c>
       <c r="B41" s="9"/>
-      <c r="C41" s="7"/>
+      <c r="C41" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12">
         <v>4.1666666666666664E-2</v>
@@ -1390,6 +1446,9 @@
         <v>29</v>
       </c>
       <c r="B42" s="9"/>
+      <c r="C42" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12">
         <v>0</v>
@@ -1404,6 +1463,9 @@
         <v>30</v>
       </c>
       <c r="B43" s="9"/>
+      <c r="C43" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E43" s="12">
         <v>0</v>
       </c>
@@ -1421,19 +1483,19 @@
         <v>0</v>
       </c>
       <c r="C44" s="13">
-        <f t="shared" ref="C44" si="20">SUM(C38:C43)*24</f>
-        <v>0</v>
+        <f t="shared" ref="C44" si="22">SUM(C38:C43)*24</f>
+        <v>8</v>
       </c>
       <c r="D44" s="13">
-        <f t="shared" ref="D44" si="21">SUM(D38:D43)*24</f>
+        <f t="shared" ref="D44" si="23">SUM(D38:D43)*24</f>
         <v>0</v>
       </c>
       <c r="E44" s="13">
-        <f t="shared" ref="E44" si="22">SUM(E38:E43)*24</f>
+        <f t="shared" ref="E44" si="24">SUM(E38:E43)*24</f>
         <v>5.9999999999999991</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" ref="F44" si="23">SUM(F38:F43)*24</f>
+        <f t="shared" ref="F44" si="25">SUM(F38:F43)*24</f>
         <v>0</v>
       </c>
       <c r="G44" s="13">
@@ -1441,11 +1503,11 @@
         <v>5.5</v>
       </c>
       <c r="H44" s="13">
-        <f t="shared" ref="H44" si="24">SUM(H38:H43)*24</f>
+        <f t="shared" ref="H44" si="26">SUM(H38:H43)*24</f>
         <v>0</v>
       </c>
       <c r="I44" s="13">
-        <f t="shared" ref="I44" si="25">SUM(I38:I43)*24</f>
+        <f t="shared" ref="I44" si="27">SUM(I38:I43)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1467,7 +1529,9 @@
         <v>8</v>
       </c>
       <c r="B46" s="9"/>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D46" s="7"/>
       <c r="E46" s="12">
         <v>4.1666666666666664E-2</v>
@@ -1482,7 +1546,9 @@
         <v>9</v>
       </c>
       <c r="B47" s="9"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D47" s="7"/>
       <c r="E47" s="12">
         <v>0.16666666666666666</v>
@@ -1497,7 +1563,9 @@
         <v>17</v>
       </c>
       <c r="B48" s="9"/>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="D48" s="12"/>
       <c r="E48" s="7">
         <v>0</v>
@@ -1512,6 +1580,9 @@
         <v>19</v>
       </c>
       <c r="B49" s="9"/>
+      <c r="C49" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12">
         <v>0</v>
@@ -1526,6 +1597,9 @@
         <v>18</v>
       </c>
       <c r="B50" s="9"/>
+      <c r="C50" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="E50" s="12">
         <v>0</v>
       </c>
@@ -1536,160 +1610,191 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12">
+        <v>0</v>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="13">
-        <f>SUM(B45:B50)*24</f>
-        <v>0</v>
-      </c>
-      <c r="C51" s="13">
-        <f t="shared" ref="C51" si="26">SUM(C45:C50)*24</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="13">
-        <f t="shared" ref="D51" si="27">SUM(D45:D50)*24</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="13">
-        <f t="shared" ref="E51" si="28">SUM(E45:E50)*24</f>
+      <c r="B52" s="13">
+        <f>SUM(B45:B51)*24</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="13">
+        <f>SUM(C45:C51)*24</f>
+        <v>8.1666666666666679</v>
+      </c>
+      <c r="D52" s="12">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E52" s="13">
+        <f>SUM(E45:E51)*24</f>
         <v>5</v>
       </c>
-      <c r="F51" s="13">
-        <f t="shared" ref="F51" si="29">SUM(F45:F50)*24</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="13">
-        <f>SUM(G46:G50)*24</f>
-        <v>5</v>
-      </c>
-      <c r="H51" s="13">
-        <f t="shared" ref="H51" si="30">SUM(H45:H50)*24</f>
-        <v>0</v>
-      </c>
-      <c r="I51" s="13">
-        <f t="shared" ref="I51" si="31">SUM(I45:I50)*24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="F52" s="13">
+        <f>SUM(F45:F51)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="13">
+        <f>SUM(G46:G51)*24</f>
+        <v>5.9999999999999991</v>
+      </c>
+      <c r="H52" s="13">
+        <f>SUM(H45:H51)*24</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="13">
+        <f>SUM(I45:I51)*24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="B53" s="8"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="12">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G53" s="12">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I53" s="12"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D54" s="7"/>
-      <c r="E54" s="7">
-        <v>0</v>
+      <c r="E54" s="12">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="G54" s="12">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I54" s="12"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B55" s="9"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12">
-        <v>6.25E-2</v>
+      <c r="C55" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7">
+        <v>0</v>
       </c>
       <c r="G55" s="12">
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B56" s="9"/>
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G56" s="12">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B57" s="9"/>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="D57" s="12"/>
       <c r="E57" s="12">
         <v>0</v>
       </c>
       <c r="G57" s="12">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I57" s="12"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="G58" s="12">
+        <v>0</v>
+      </c>
+      <c r="I58" s="12"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="13">
-        <f>SUM(B52:B57)*24</f>
-        <v>0</v>
-      </c>
-      <c r="C58" s="13">
-        <f t="shared" ref="C58" si="32">SUM(C52:C57)*24</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="13">
-        <f t="shared" ref="D58" si="33">SUM(D52:D57)*24</f>
-        <v>0</v>
-      </c>
-      <c r="E58" s="13">
-        <f t="shared" ref="E58" si="34">SUM(E52:E57)*24</f>
+      <c r="B59" s="13">
+        <f>SUM(B54:B58)*24</f>
+        <v>0</v>
+      </c>
+      <c r="C59" s="13">
+        <f>SUM(C54:C58)*24</f>
+        <v>5.5</v>
+      </c>
+      <c r="D59" s="13">
+        <f>SUM(D54:D58)*24</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="13">
+        <f>SUM(E54:E58)*24</f>
         <v>2.5</v>
       </c>
-      <c r="F58" s="13">
-        <f t="shared" ref="F58" si="35">SUM(F52:F57)*24</f>
-        <v>0</v>
-      </c>
-      <c r="G58" s="13">
-        <f>SUM(G53:G57)*24</f>
-        <v>4</v>
-      </c>
-      <c r="H58" s="13">
-        <f t="shared" ref="H58" si="36">SUM(H52:H57)*24</f>
-        <v>0</v>
-      </c>
-      <c r="I58" s="13">
-        <f t="shared" ref="I58" si="37">SUM(I52:I57)*24</f>
+      <c r="F59" s="13">
+        <f>SUM(F54:F58)*24</f>
+        <v>0</v>
+      </c>
+      <c r="G59" s="13">
+        <f>SUM(G55:G58)*24</f>
+        <v>3</v>
+      </c>
+      <c r="H59" s="13">
+        <f>SUM(H54:H58)*24</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="13">
+        <f>SUM(I54:I58)*24</f>
         <v>0</v>
       </c>
     </row>
@@ -1698,42 +1803,44 @@
         <v>27</v>
       </c>
       <c r="B60" s="14">
-        <f>SUM(B58,B51,B44,B37,B30,B23,B16,B9)</f>
+        <f>SUM(B59,B52,B44,B37,B30,B23,B16,B9)</f>
         <v>11.25</v>
       </c>
       <c r="C60" s="14">
-        <f t="shared" ref="C60:I60" si="38">SUM(C58,C51,C44,C37,C30,C23,C16,C9)</f>
-        <v>13.333333333333332</v>
+        <f>SUM(C59,C52,C44,C37,C30,C23,C16,C9)</f>
+        <v>50.416666666666671</v>
       </c>
       <c r="D60" s="14">
-        <f t="shared" si="38"/>
-        <v>18.833333333333332</v>
+        <f>SUM(D59,D52,D52,D44,D37,D30,D23,D16,D9)</f>
+        <v>18.916666666666664</v>
       </c>
       <c r="E60" s="14">
-        <f t="shared" si="38"/>
+        <f>SUM(E59,E52,E44,E37,E30,E23,E16,E9)</f>
         <v>43</v>
       </c>
       <c r="F60" s="14">
-        <f t="shared" si="38"/>
+        <f>SUM(F59,F52,F44,F37,F30,F23,F16,F9)</f>
         <v>5.1666666666666661</v>
       </c>
       <c r="G60" s="14">
-        <f>SUM(G9:G16:G23:G30:G37:G44:G51:G58)</f>
-        <v>45.229166666666664</v>
+        <f>SUM(G59,G52,G44,G37,G30,G23,G16,G9)</f>
+        <v>43.666666666666664</v>
       </c>
       <c r="H60" s="14">
-        <f t="shared" si="38"/>
+        <f>SUM(H59,H52,H44,H37,H30,H23,H16,H9)</f>
         <v>5.75</v>
       </c>
       <c r="I60" s="14">
-        <f t="shared" si="38"/>
+        <f>SUM(I59,I52,I44,I37,I30,I23,I16,I9)</f>
         <v>21.833333333333336</v>
       </c>
     </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="14"/>
+      <c r="C61" s="16"/>
+    </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G62" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B62" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uren Wesley ook toegevoegd
</commit_message>
<xml_diff>
--- a/Urendeclaratie.xlsx
+++ b/Urendeclaratie.xlsx
@@ -577,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +870,9 @@
       <c r="G11" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H11" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I11" s="12">
         <v>0</v>
       </c>
@@ -893,6 +896,9 @@
       <c r="G12" s="12">
         <v>0.16666666666666666</v>
       </c>
+      <c r="H12" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I12" s="12">
         <v>0.16666666666666666</v>
       </c>
@@ -916,6 +922,9 @@
       <c r="G13" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="H13" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I13" s="12">
         <v>1.3888888888888888E-2</v>
       </c>
@@ -939,6 +948,9 @@
       <c r="G14" s="12">
         <v>0</v>
       </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
       <c r="I14" s="12">
         <v>0.25</v>
       </c>
@@ -957,6 +969,9 @@
       <c r="G15" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
       <c r="I15" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -991,7 +1006,7 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I16" s="13">
         <f t="shared" si="3"/>
@@ -1030,6 +1045,9 @@
       <c r="G18" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H18" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I18" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1053,6 +1071,9 @@
       <c r="G19" s="12">
         <v>0.16666666666666666</v>
       </c>
+      <c r="H19" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I19" s="12">
         <v>0</v>
       </c>
@@ -1074,6 +1095,9 @@
       <c r="G20" s="12">
         <v>0</v>
       </c>
+      <c r="H20" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="I20" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1097,6 +1121,9 @@
       <c r="G21" s="12">
         <v>0</v>
       </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
       <c r="I21" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1117,6 +1144,9 @@
       <c r="G22" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H22" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I22" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1151,7 +1181,7 @@
       </c>
       <c r="H23" s="13">
         <f t="shared" ref="H23" si="8">SUM(H17:H22)*24</f>
-        <v>0</v>
+        <v>5.6666666666666661</v>
       </c>
       <c r="I23" s="13">
         <f t="shared" ref="I23" si="9">SUM(I17:I22)*24</f>
@@ -1188,6 +1218,9 @@
       <c r="G25" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H25" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I25" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1209,6 +1242,9 @@
       <c r="G26" s="12">
         <v>0</v>
       </c>
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
       <c r="I26" s="12">
         <v>0</v>
       </c>
@@ -1230,6 +1266,9 @@
       <c r="G27" s="12">
         <v>0</v>
       </c>
+      <c r="H27" s="7">
+        <v>0</v>
+      </c>
       <c r="I27" s="12">
         <v>0</v>
       </c>
@@ -1251,6 +1290,9 @@
       <c r="G28" s="12">
         <v>0</v>
       </c>
+      <c r="H28" s="7">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="I28" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1271,6 +1313,9 @@
       <c r="G29" s="12">
         <v>0.10416666666666667</v>
       </c>
+      <c r="H29" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="I29" s="12">
         <v>0</v>
       </c>
@@ -1305,7 +1350,7 @@
       </c>
       <c r="H30" s="13">
         <f t="shared" ref="H30" si="14">SUM(H24:H29)*24</f>
-        <v>0</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="I30" s="13">
         <f t="shared" ref="I30" si="15">SUM(I24:I29)*24</f>
@@ -1342,6 +1387,9 @@
       <c r="G32" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H32" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I32" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1363,6 +1411,9 @@
       <c r="G33" s="12">
         <v>0.16666666666666666</v>
       </c>
+      <c r="H33" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I33" s="12">
         <v>0</v>
       </c>
@@ -1384,6 +1435,9 @@
       <c r="G34" s="12">
         <v>0</v>
       </c>
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
       <c r="I34" s="12">
         <v>0</v>
       </c>
@@ -1405,6 +1459,9 @@
       <c r="G35" s="12">
         <v>0</v>
       </c>
+      <c r="H35" s="7">
+        <v>0</v>
+      </c>
       <c r="I35" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -1425,6 +1482,9 @@
       <c r="G36" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H36" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I36" s="12">
         <v>0</v>
       </c>
@@ -1459,7 +1519,7 @@
       </c>
       <c r="H37" s="13">
         <f t="shared" ref="H37" si="20">SUM(H31:H36)*24</f>
-        <v>0</v>
+        <v>5.9999999999999991</v>
       </c>
       <c r="I37" s="13">
         <f t="shared" ref="I37" si="21">SUM(I31:I36)*24</f>
@@ -1496,6 +1556,9 @@
       <c r="G39" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H39" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I39" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1517,6 +1580,9 @@
       <c r="G40" s="12">
         <v>0.16666666666666666</v>
       </c>
+      <c r="H40" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I40" s="12">
         <v>0.16666666666666666</v>
       </c>
@@ -1538,6 +1604,9 @@
       <c r="G41" s="12">
         <v>0</v>
       </c>
+      <c r="H41" s="7">
+        <v>0</v>
+      </c>
       <c r="I41" s="12">
         <v>0</v>
       </c>
@@ -1559,6 +1628,9 @@
       <c r="G42" s="12">
         <v>0</v>
       </c>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
       <c r="I42" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -1579,6 +1651,9 @@
       <c r="G43" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
+      <c r="H43" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I43" s="12">
         <v>0</v>
       </c>
@@ -1613,7 +1688,7 @@
       </c>
       <c r="H44" s="13">
         <f t="shared" ref="H44" si="26">SUM(H38:H43)*24</f>
-        <v>0</v>
+        <v>5.9999999999999991</v>
       </c>
       <c r="I44" s="13">
         <f t="shared" ref="I44" si="27">SUM(I38:I43)*24</f>
@@ -1650,6 +1725,9 @@
       <c r="G46" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H46" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I46" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1671,6 +1749,9 @@
       <c r="G47" s="12">
         <v>0.16666666666666666</v>
       </c>
+      <c r="H47" s="7">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="I47" s="12">
         <v>0.16666666666666666</v>
       </c>
@@ -1692,6 +1773,9 @@
       <c r="G48" s="12">
         <v>0</v>
       </c>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
       <c r="I48" s="12">
         <v>0</v>
       </c>
@@ -1713,6 +1797,9 @@
       <c r="G49" s="12">
         <v>0</v>
       </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
       <c r="I49" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -1733,6 +1820,9 @@
       <c r="G50" s="12">
         <v>0</v>
       </c>
+      <c r="H50" s="7">
+        <v>0</v>
+      </c>
       <c r="I50" s="12">
         <v>0</v>
       </c>
@@ -1755,7 +1845,9 @@
       <c r="G51" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="H51" s="12"/>
+      <c r="H51" s="7">
+        <v>1</v>
+      </c>
       <c r="I51" s="9">
         <v>0</v>
       </c>
@@ -1789,7 +1881,7 @@
       </c>
       <c r="H52" s="13">
         <f>SUM(H45:H51)*24</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I52" s="13">
         <f>SUM(I45:I51)*24</f>
@@ -1826,6 +1918,9 @@
       <c r="G54" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="H54" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I54" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -1847,6 +1942,9 @@
       <c r="G55" s="12">
         <v>0</v>
       </c>
+      <c r="H55" s="7">
+        <v>0</v>
+      </c>
       <c r="I55" s="12">
         <v>0</v>
       </c>
@@ -1868,6 +1966,9 @@
       <c r="G56" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
+      <c r="H56" s="7">
+        <v>6.25E-2</v>
+      </c>
       <c r="I56" s="12">
         <v>0.10416666666666667</v>
       </c>
@@ -1889,6 +1990,9 @@
       <c r="G57" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
+      <c r="H57" s="7">
+        <v>0</v>
+      </c>
       <c r="I57" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -1910,6 +2014,9 @@
       <c r="G58" s="12">
         <v>0</v>
       </c>
+      <c r="H58" s="7">
+        <v>0</v>
+      </c>
       <c r="I58" s="12">
         <v>0</v>
       </c>
@@ -1944,7 +2051,7 @@
       </c>
       <c r="H59" s="17">
         <f>SUM(H54:H58)*24</f>
-        <v>0</v>
+        <v>3.4999999999999996</v>
       </c>
       <c r="I59" s="17">
         <f>SUM(I54:I58)*24</f>
@@ -1981,7 +2088,7 @@
       </c>
       <c r="H60" s="14">
         <f>SUM(H59,H52,H44,H37,H30,H23,H16,H9)</f>
-        <v>5.75</v>
+        <v>63.083333333333329</v>
       </c>
       <c r="I60" s="14">
         <f>SUM(I59,I52,I44,I37,I30,I23,I16,I9)</f>
@@ -1993,35 +2100,35 @@
         <v>33</v>
       </c>
       <c r="B61" s="14">
-        <f>SUM(B55,B47,B40,B33,B26,B19,B12,B4)*24</f>
+        <f t="shared" ref="B61:I61" si="28">SUM(B55,B47,B40,B33,B26,B19,B12,B4)*24</f>
         <v>23.999999999999996</v>
       </c>
       <c r="C61" s="14">
-        <f>SUM(C55,C47,C40,C33,C26,C19,C12,C4)*24</f>
+        <f t="shared" si="28"/>
         <v>23.999999999999996</v>
       </c>
       <c r="D61" s="14">
-        <f>SUM(D55,D47,D40,D33,D26,D19,D12,D4)*24</f>
+        <f t="shared" si="28"/>
         <v>12</v>
       </c>
       <c r="E61" s="14">
-        <f>SUM(E55,E47,E40,E33,E26,E19,E12,E4)*24</f>
+        <f t="shared" si="28"/>
         <v>23.999999999999996</v>
       </c>
       <c r="F61" s="14">
-        <f>SUM(F55,F47,F40,F33,F26,F19,F12,F4)*24</f>
+        <f t="shared" si="28"/>
         <v>4</v>
       </c>
       <c r="G61" s="14">
-        <f>SUM(G55,G47,G40,G33,G26,G19,G12,G4)*24</f>
+        <f t="shared" si="28"/>
         <v>23.999999999999996</v>
       </c>
       <c r="H61" s="14">
-        <f>SUM(H55,H47,H40,H33,H26,H19,H12,H4)*24</f>
-        <v>4</v>
+        <f t="shared" si="28"/>
+        <v>23.999999999999996</v>
       </c>
       <c r="I61" s="14">
-        <f>SUM(I55,I47,I40,I33,I26,I19,I12,I4)*24</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
     </row>
@@ -2034,31 +2141,31 @@
         <v>21.750000000000004</v>
       </c>
       <c r="C62" s="14">
-        <f t="shared" ref="C62:I62" si="28">C60-C61</f>
+        <f t="shared" ref="C62:I62" si="29">C60-C61</f>
         <v>24.416666666666675</v>
       </c>
       <c r="D62" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>6.9166666666666643</v>
       </c>
       <c r="E62" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>20.000000000000004</v>
       </c>
       <c r="F62" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.1666666666666661</v>
       </c>
       <c r="G62" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>19.666666666666668</v>
       </c>
       <c r="H62" s="14">
-        <f t="shared" si="28"/>
-        <v>1.75</v>
+        <f t="shared" si="29"/>
+        <v>39.083333333333329</v>
       </c>
       <c r="I62" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>31.833333333333336</v>
       </c>
     </row>

</xml_diff>